<commit_message>
Added analysts and statistics for KVPP
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/kvpp.xlsx
+++ b/storage/app/excel/templates/kvpp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\business-processes\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC8269-6B2C-4C1B-83F5-CF8CE248FFF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E91E5F2-221A-4AC3-BFFF-2E31277D8356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Страна</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Нвои</t>
+  </si>
+  <si>
+    <t>Аналитик</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,12 +519,12 @@
     <col min="16" max="16" width="13.5703125" customWidth="1"/>
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
     <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" customWidth="1"/>
-    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -577,12 +580,15 @@
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>